<commit_message>
Fix crawl order error.
</commit_message>
<xml_diff>
--- a/kariwaza.xlsx
+++ b/kariwaza.xlsx
@@ -133,6 +133,18 @@
     <t>集★7汝ノチカラヲ、見セテミヨ</t>
   </si>
   <si>
+    <t>ムーンブレイク</t>
+  </si>
+  <si>
+    <t>村★7調査隊初陣！遺群嶺の桃毛獣 または 集★7その腕前、噂通りかしら…？</t>
+  </si>
+  <si>
+    <t>G★2鎌蟹の狩猟をさせてやるぜ！</t>
+  </si>
+  <si>
+    <t>G★4巨獣の進攻</t>
+  </si>
+  <si>
     <t>太刀</t>
   </si>
   <si>
@@ -160,6 +172,15 @@
     <t>集★7グランド・ハンター・ゲーム</t>
   </si>
   <si>
+    <t>妖刀羅刹</t>
+  </si>
+  <si>
+    <t>G★2空の家族・空路を守るッス</t>
+  </si>
+  <si>
+    <t>G★4風薫る密林</t>
+  </si>
+  <si>
     <t>片手剣</t>
   </si>
   <si>
@@ -187,6 +208,15 @@
     <t>集★6スリルとショックの氷海ツアー</t>
   </si>
   <si>
+    <t>混沌の刃薬</t>
+  </si>
+  <si>
+    <t>G★2密林のナルガクルガと対峙せよ</t>
+  </si>
+  <si>
+    <t>G★4金と銀がもたらす悲哀</t>
+  </si>
+  <si>
     <t>双剣</t>
   </si>
   <si>
@@ -211,6 +241,12 @@
     <t>集★7憤怒の雄叫び</t>
   </si>
   <si>
+    <t>ラセンザン</t>
+  </si>
+  <si>
+    <t>G★4焦電</t>
+  </si>
+  <si>
     <t>ハンマー</t>
   </si>
   <si>
@@ -238,6 +274,15 @@
     <t>集★7勇猛果敢なブレイブタスク</t>
   </si>
   <si>
+    <t>インパクトプルス</t>
+  </si>
+  <si>
+    <t>G★2……欲するならば資格を示して</t>
+  </si>
+  <si>
+    <t>G★4砂漠の死闘と未来</t>
+  </si>
+  <si>
     <t>狩猟笛</t>
   </si>
   <si>
@@ -262,6 +307,12 @@
     <t>集★5毒、麻痺、混乱にご用心！</t>
   </si>
   <si>
+    <t>アニマートハイ</t>
+  </si>
+  <si>
+    <t>G★4狩魂よ砂中に眠れ</t>
+  </si>
+  <si>
     <t>ランス</t>
   </si>
   <si>
@@ -289,6 +340,15 @@
     <t>集★6原生林の曲者たち</t>
   </si>
   <si>
+    <t>治癒の盾</t>
+  </si>
+  <si>
+    <t>G★2依頼委託：火山の岩竜</t>
+  </si>
+  <si>
+    <t>G★4シャル・ウィ・ダンス？</t>
+  </si>
+  <si>
     <t>ガンランス</t>
   </si>
   <si>
@@ -313,6 +373,12 @@
     <t>集★7熱気で熱狂！炎の軍勢！</t>
   </si>
   <si>
+    <t>AAフレア</t>
+  </si>
+  <si>
+    <t>G★4死神は鎧をまとう</t>
+  </si>
+  <si>
     <t>スラッシュアックス</t>
   </si>
   <si>
@@ -337,6 +403,15 @@
     <t>集★6燃えたぎれ！火山の熱闘！！</t>
   </si>
   <si>
+    <t>テンペストアクス</t>
+  </si>
+  <si>
+    <t>G★2二人で特訓、成果は山分け</t>
+  </si>
+  <si>
+    <t>G★4騎士と氷海の決闘</t>
+  </si>
+  <si>
     <t>チャージアックス</t>
   </si>
   <si>
@@ -361,6 +436,12 @@
     <t>集★6飛竜たちの乱舞</t>
   </si>
   <si>
+    <t>チェインソーサー</t>
+  </si>
+  <si>
+    <t>G★4無心にて森羅万象を断つ</t>
+  </si>
+  <si>
     <t>操虫棍</t>
   </si>
   <si>
@@ -385,6 +466,12 @@
     <t>集★6沼地の狂騒楽団</t>
   </si>
   <si>
+    <t>覚蟲強化</t>
+  </si>
+  <si>
+    <t>G★4天を廻りて、冥界に堕つ</t>
+  </si>
+  <si>
     <t>ライトボウガン</t>
   </si>
   <si>
@@ -409,6 +496,15 @@
     <t>集★7住めば都の闘技場暮らし</t>
   </si>
   <si>
+    <t>チャージショット</t>
+  </si>
+  <si>
+    <t>G★2閃きへの1ピースを求めて</t>
+  </si>
+  <si>
+    <t>G★4溶岩島で爆ぜる砕光</t>
+  </si>
+  <si>
     <t>ヘビィボウガン</t>
   </si>
   <si>
@@ -436,6 +532,12 @@
     <t>集★6地底火山に響く侵略の足音</t>
   </si>
   <si>
+    <t>射突型裂孔弾</t>
+  </si>
+  <si>
+    <t>G★4戦慄の遺群嶺</t>
+  </si>
+  <si>
     <t>弓</t>
   </si>
   <si>
@@ -458,108 +560,6 @@
   </si>
   <si>
     <t>集★6ワイルドバレット</t>
-  </si>
-  <si>
-    <t>ムーンブレイク</t>
-  </si>
-  <si>
-    <t>村★7調査隊初陣！遺群嶺の桃毛獣 または 集★7その腕前、噂通りかしら…？</t>
-  </si>
-  <si>
-    <t>G★2鎌蟹の狩猟をさせてやるぜ！</t>
-  </si>
-  <si>
-    <t>G★4巨獣の進攻</t>
-  </si>
-  <si>
-    <t>妖刀羅刹</t>
-  </si>
-  <si>
-    <t>G★2空の家族・空路を守るッス</t>
-  </si>
-  <si>
-    <t>G★4風薫る密林</t>
-  </si>
-  <si>
-    <t>混沌の刃薬</t>
-  </si>
-  <si>
-    <t>G★2密林のナルガクルガと対峙せよ</t>
-  </si>
-  <si>
-    <t>G★4金と銀がもたらす悲哀</t>
-  </si>
-  <si>
-    <t>ラセンザン</t>
-  </si>
-  <si>
-    <t>G★4焦電</t>
-  </si>
-  <si>
-    <t>インパクトプルス</t>
-  </si>
-  <si>
-    <t>G★2……欲するならば資格を示して</t>
-  </si>
-  <si>
-    <t>G★4砂漠の死闘と未来</t>
-  </si>
-  <si>
-    <t>アニマートハイ</t>
-  </si>
-  <si>
-    <t>G★4狩魂よ砂中に眠れ</t>
-  </si>
-  <si>
-    <t>治癒の盾</t>
-  </si>
-  <si>
-    <t>G★2依頼委託：火山の岩竜</t>
-  </si>
-  <si>
-    <t>G★4シャル・ウィ・ダンス？</t>
-  </si>
-  <si>
-    <t>AAフレア</t>
-  </si>
-  <si>
-    <t>G★4死神は鎧をまとう</t>
-  </si>
-  <si>
-    <t>テンペストアクス</t>
-  </si>
-  <si>
-    <t>G★2二人で特訓、成果は山分け</t>
-  </si>
-  <si>
-    <t>G★4騎士と氷海の決闘</t>
-  </si>
-  <si>
-    <t>チェインソーサー</t>
-  </si>
-  <si>
-    <t>G★4無心にて森羅万象を断つ</t>
-  </si>
-  <si>
-    <t>覚蟲強化</t>
-  </si>
-  <si>
-    <t>G★4天を廻りて、冥界に堕つ</t>
-  </si>
-  <si>
-    <t>チャージショット</t>
-  </si>
-  <si>
-    <t>G★2閃きへの1ピースを求めて</t>
-  </si>
-  <si>
-    <t>G★4溶岩島で爆ぜる砕光</t>
-  </si>
-  <si>
-    <t>射突型裂孔弾</t>
-  </si>
-  <si>
-    <t>G★4戦慄の遺群嶺</t>
   </si>
   <si>
     <t>身躱し射法</t>
@@ -1185,133 +1185,133 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
         <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
       <c r="C22" t="s">
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
       <c r="C23" t="s">
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
         <v>49</v>
@@ -1320,12 +1320,12 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
         <v>49</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
         <v>49</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
         <v>52</v>
@@ -1362,12 +1362,12 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
         <v>52</v>
@@ -1376,12 +1376,12 @@
         <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
         <v>52</v>
@@ -1390,57 +1390,57 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
         <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
         <v>28</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
         <v>28</v>
@@ -1465,24 +1465,24 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
         <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -1493,80 +1493,80 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
         <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
         <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
         <v>27</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>28</v>
       </c>
       <c r="D46" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
         <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
         <v>27</v>
@@ -1577,10 +1577,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
         <v>28</v>
@@ -1591,24 +1591,24 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
         <v>30</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
         <v>27</v>
@@ -1619,38 +1619,38 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C52" t="s">
         <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C53" t="s">
         <v>30</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
         <v>27</v>
@@ -1661,35 +1661,35 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C55" t="s">
         <v>28</v>
       </c>
       <c r="D55" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C56" t="s">
         <v>30</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B57" t="s">
         <v>75</v>
@@ -1698,12 +1698,12 @@
         <v>27</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
         <v>75</v>
@@ -1712,12 +1712,12 @@
         <v>28</v>
       </c>
       <c r="D58" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
         <v>75</v>
@@ -1726,57 +1726,57 @@
         <v>30</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C60" t="s">
         <v>27</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C61" t="s">
         <v>28</v>
       </c>
       <c r="D61" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
         <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
         <v>27</v>
@@ -1787,35 +1787,35 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C64" t="s">
         <v>28</v>
       </c>
       <c r="D64" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
         <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
         <v>83</v>
@@ -1824,12 +1824,12 @@
         <v>27</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B67" t="s">
         <v>83</v>
@@ -1838,12 +1838,12 @@
         <v>28</v>
       </c>
       <c r="D67" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
         <v>83</v>
@@ -1852,211 +1852,211 @@
         <v>30</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C69" t="s">
         <v>27</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C70" t="s">
         <v>28</v>
       </c>
       <c r="D70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C71" t="s">
         <v>30</v>
       </c>
       <c r="D71" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
         <v>27</v>
       </c>
       <c r="D72" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
       </c>
       <c r="D73" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C74" t="s">
         <v>30</v>
       </c>
       <c r="D74" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" t="s">
         <v>91</v>
       </c>
-      <c r="B75" t="s">
-        <v>92</v>
-      </c>
       <c r="C75" t="s">
         <v>27</v>
       </c>
       <c r="D75" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" t="s">
         <v>91</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
+        <v>28</v>
+      </c>
+      <c r="D76" t="s">
         <v>92</v>
-      </c>
-      <c r="C76" t="s">
-        <v>28</v>
-      </c>
-      <c r="D76" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77" t="s">
         <v>91</v>
       </c>
-      <c r="B77" t="s">
-        <v>92</v>
-      </c>
       <c r="C77" t="s">
         <v>30</v>
       </c>
       <c r="D77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
         <v>27</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B79" t="s">
+        <v>94</v>
+      </c>
+      <c r="C79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" t="s">
         <v>95</v>
-      </c>
-      <c r="C79" t="s">
-        <v>28</v>
-      </c>
-      <c r="D79" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
         <v>30</v>
       </c>
       <c r="D80" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B81" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C81" t="s">
         <v>27</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B82" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C82" t="s">
         <v>28</v>
       </c>
       <c r="D82" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C83" t="s">
         <v>30</v>
@@ -2104,7 +2104,7 @@
         <v>30</v>
       </c>
       <c r="D86" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2112,13 +2112,13 @@
         <v>99</v>
       </c>
       <c r="B87" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C87" t="s">
         <v>27</v>
       </c>
       <c r="D87" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2126,13 +2126,13 @@
         <v>99</v>
       </c>
       <c r="B88" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C88" t="s">
         <v>28</v>
       </c>
       <c r="D88" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2140,13 +2140,13 @@
         <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C89" t="s">
         <v>30</v>
       </c>
       <c r="D89" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2154,13 +2154,13 @@
         <v>99</v>
       </c>
       <c r="B90" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C90" t="s">
         <v>27</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2168,13 +2168,13 @@
         <v>99</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C91" t="s">
         <v>28</v>
       </c>
       <c r="D91" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2182,18 +2182,18 @@
         <v>99</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
         <v>30</v>
       </c>
       <c r="D92" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B93" t="s">
         <v>108</v>
@@ -2202,12 +2202,12 @@
         <v>27</v>
       </c>
       <c r="D93" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B94" t="s">
         <v>108</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B95" t="s">
         <v>108</v>
@@ -2235,91 +2235,91 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
         <v>27</v>
       </c>
       <c r="D96" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B97" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
       </c>
       <c r="D97" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C98" t="s">
         <v>30</v>
       </c>
       <c r="D98" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B99" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C99" t="s">
         <v>27</v>
       </c>
       <c r="D99" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B100" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
       </c>
       <c r="D100" t="s">
-        <v>113</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B101" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C101" t="s">
         <v>30</v>
       </c>
       <c r="D101" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B102" t="s">
         <v>116</v>
@@ -2328,12 +2328,12 @@
         <v>27</v>
       </c>
       <c r="D102" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B103" t="s">
         <v>116</v>
@@ -2342,12 +2342,12 @@
         <v>28</v>
       </c>
       <c r="D103" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B104" t="s">
         <v>116</v>
@@ -2356,337 +2356,337 @@
         <v>30</v>
       </c>
       <c r="D104" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C105" t="s">
         <v>27</v>
       </c>
       <c r="D105" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B106" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C106" t="s">
         <v>28</v>
       </c>
       <c r="D106" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B107" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
         <v>30</v>
       </c>
       <c r="D107" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C108" t="s">
         <v>27</v>
       </c>
       <c r="D108" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C109" t="s">
         <v>28</v>
       </c>
       <c r="D109" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B110" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C110" t="s">
         <v>30</v>
       </c>
       <c r="D110" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
+        <v>121</v>
+      </c>
+      <c r="B111" t="s">
         <v>123</v>
       </c>
-      <c r="B111" t="s">
-        <v>124</v>
-      </c>
       <c r="C111" t="s">
         <v>27</v>
       </c>
       <c r="D111" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
+        <v>121</v>
+      </c>
+      <c r="B112" t="s">
         <v>123</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112" t="s">
         <v>124</v>
-      </c>
-      <c r="C112" t="s">
-        <v>28</v>
-      </c>
-      <c r="D112" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
+        <v>121</v>
+      </c>
+      <c r="B113" t="s">
         <v>123</v>
       </c>
-      <c r="B113" t="s">
-        <v>124</v>
-      </c>
       <c r="C113" t="s">
         <v>30</v>
       </c>
       <c r="D113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B114" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C114" t="s">
         <v>27</v>
       </c>
       <c r="D114" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B115" t="s">
+        <v>126</v>
+      </c>
+      <c r="C115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" t="s">
         <v>127</v>
-      </c>
-      <c r="C115" t="s">
-        <v>28</v>
-      </c>
-      <c r="D115" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B116" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C116" t="s">
         <v>30</v>
       </c>
       <c r="D116" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B117" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C117" t="s">
         <v>27</v>
       </c>
       <c r="D117" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C118" t="s">
         <v>28</v>
       </c>
       <c r="D118" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C119" t="s">
         <v>30</v>
       </c>
       <c r="D119" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B120" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C120" t="s">
         <v>27</v>
       </c>
       <c r="D120" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B121" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C121" t="s">
         <v>28</v>
       </c>
       <c r="D121" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B122" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C122" t="s">
         <v>30</v>
       </c>
       <c r="D122" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C123" t="s">
         <v>27</v>
       </c>
       <c r="D123" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B124" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
       </c>
       <c r="D124" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B125" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C125" t="s">
         <v>30</v>
       </c>
       <c r="D125" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C126" t="s">
         <v>27</v>
       </c>
       <c r="D126" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B127" t="s">
+        <v>137</v>
+      </c>
+      <c r="C127" t="s">
+        <v>28</v>
+      </c>
+      <c r="D127" t="s">
         <v>138</v>
-      </c>
-      <c r="C127" t="s">
-        <v>28</v>
-      </c>
-      <c r="D127" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B128" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C128" t="s">
         <v>30</v>
@@ -2697,49 +2697,49 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
+        <v>132</v>
+      </c>
+      <c r="B129" t="s">
         <v>140</v>
       </c>
-      <c r="B129" t="s">
-        <v>141</v>
-      </c>
       <c r="C129" t="s">
         <v>27</v>
       </c>
       <c r="D129" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" t="s">
         <v>140</v>
       </c>
-      <c r="B130" t="s">
-        <v>141</v>
-      </c>
       <c r="C130" t="s">
         <v>28</v>
       </c>
       <c r="D130" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" t="s">
         <v>140</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
+        <v>30</v>
+      </c>
+      <c r="D131" t="s">
         <v>141</v>
-      </c>
-      <c r="C131" t="s">
-        <v>30</v>
-      </c>
-      <c r="D131" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B132" t="s">
         <v>143</v>
@@ -2748,12 +2748,12 @@
         <v>27</v>
       </c>
       <c r="D132" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B133" t="s">
         <v>143</v>
@@ -2762,12 +2762,12 @@
         <v>28</v>
       </c>
       <c r="D133" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B134" t="s">
         <v>143</v>
@@ -2776,15 +2776,15 @@
         <v>30</v>
       </c>
       <c r="D134" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B135" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C135" t="s">
         <v>27</v>
@@ -2795,262 +2795,262 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B136" t="s">
+        <v>144</v>
+      </c>
+      <c r="C136" t="s">
+        <v>28</v>
+      </c>
+      <c r="D136" t="s">
         <v>145</v>
-      </c>
-      <c r="C136" t="s">
-        <v>28</v>
-      </c>
-      <c r="D136" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B137" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C137" t="s">
         <v>30</v>
       </c>
       <c r="D137" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B138" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C138" t="s">
         <v>27</v>
       </c>
       <c r="D138" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B139" t="s">
+        <v>147</v>
+      </c>
+      <c r="C139" t="s">
+        <v>28</v>
+      </c>
+      <c r="D139" t="s">
         <v>148</v>
-      </c>
-      <c r="C139" t="s">
-        <v>28</v>
-      </c>
-      <c r="D139" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C140" t="s">
         <v>30</v>
       </c>
       <c r="D140" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B141" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C141" t="s">
         <v>27</v>
       </c>
       <c r="D141" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
       </c>
       <c r="D142" t="s">
-        <v>153</v>
+        <v>41</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C143" t="s">
         <v>30</v>
       </c>
       <c r="D143" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B144" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C144" t="s">
         <v>27</v>
       </c>
       <c r="D144" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B145" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C145" t="s">
         <v>28</v>
       </c>
       <c r="D145" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B146" t="s">
+        <v>153</v>
+      </c>
+      <c r="C146" t="s">
+        <v>30</v>
+      </c>
+      <c r="D146" t="s">
         <v>155</v>
-      </c>
-      <c r="C146" t="s">
-        <v>30</v>
-      </c>
-      <c r="D146" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B147" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C147" t="s">
         <v>27</v>
       </c>
       <c r="D147" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B148" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C148" t="s">
         <v>28</v>
       </c>
       <c r="D148" t="s">
-        <v>156</v>
+        <v>29</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B149" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C149" t="s">
         <v>30</v>
       </c>
       <c r="D149" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C150" t="s">
         <v>27</v>
       </c>
       <c r="D150" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C151" t="s">
         <v>28</v>
       </c>
       <c r="D151" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C152" t="s">
         <v>30</v>
       </c>
       <c r="D152" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C153" t="s">
         <v>27</v>
       </c>
       <c r="D153" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -3061,94 +3061,94 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B155" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C155" t="s">
         <v>30</v>
       </c>
       <c r="D155" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B156" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C156" t="s">
         <v>27</v>
       </c>
       <c r="D156" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B157" t="s">
+        <v>164</v>
+      </c>
+      <c r="C157" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157" t="s">
         <v>165</v>
-      </c>
-      <c r="C157" t="s">
-        <v>28</v>
-      </c>
-      <c r="D157" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B158" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C158" t="s">
         <v>30</v>
       </c>
       <c r="D158" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B159" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C159" t="s">
         <v>27</v>
       </c>
       <c r="D159" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B160" t="s">
+        <v>167</v>
+      </c>
+      <c r="C160" t="s">
+        <v>28</v>
+      </c>
+      <c r="D160" t="s">
         <v>168</v>
-      </c>
-      <c r="C160" t="s">
-        <v>28</v>
-      </c>
-      <c r="D160" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C161" t="s">
         <v>30</v>
@@ -3159,7 +3159,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B162" t="s">
         <v>170</v>
@@ -3168,12 +3168,12 @@
         <v>27</v>
       </c>
       <c r="D162" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B163" t="s">
         <v>170</v>
@@ -3182,12 +3182,12 @@
         <v>28</v>
       </c>
       <c r="D163" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B164" t="s">
         <v>170</v>
@@ -3196,54 +3196,54 @@
         <v>30</v>
       </c>
       <c r="D164" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C165" t="s">
         <v>27</v>
       </c>
       <c r="D165" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B166" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C166" t="s">
         <v>28</v>
       </c>
       <c r="D166" t="s">
-        <v>171</v>
+        <v>53</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B167" t="s">
+        <v>172</v>
+      </c>
+      <c r="C167" t="s">
+        <v>30</v>
+      </c>
+      <c r="D167" t="s">
         <v>173</v>
-      </c>
-      <c r="C167" t="s">
-        <v>30</v>
-      </c>
-      <c r="D167" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B168" t="s">
         <v>175</v>
@@ -3252,12 +3252,12 @@
         <v>27</v>
       </c>
       <c r="D168" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B169" t="s">
         <v>175</v>
@@ -3266,12 +3266,12 @@
         <v>28</v>
       </c>
       <c r="D169" t="s">
-        <v>150</v>
+        <v>29</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B170" t="s">
         <v>175</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B171" t="s">
         <v>177</v>
@@ -3294,12 +3294,12 @@
         <v>27</v>
       </c>
       <c r="D171" t="s">
-        <v>149</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B172" t="s">
         <v>177</v>
@@ -3313,7 +3313,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B173" t="s">
         <v>177</v>
@@ -3322,43 +3322,43 @@
         <v>30</v>
       </c>
       <c r="D173" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C174" t="s">
         <v>27</v>
       </c>
       <c r="D174" t="s">
-        <v>149</v>
+        <v>33</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B175" t="s">
+        <v>179</v>
+      </c>
+      <c r="C175" t="s">
+        <v>28</v>
+      </c>
+      <c r="D175" t="s">
         <v>180</v>
-      </c>
-      <c r="C175" t="s">
-        <v>28</v>
-      </c>
-      <c r="D175" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C176" t="s">
         <v>30</v>
@@ -3369,7 +3369,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B177" t="s">
         <v>182</v>
@@ -3378,12 +3378,12 @@
         <v>27</v>
       </c>
       <c r="D177" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B178" t="s">
         <v>182</v>
@@ -3392,12 +3392,12 @@
         <v>28</v>
       </c>
       <c r="D178" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B179" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Translation of kariwaza information except condition.
</commit_message>
<xml_diff>
--- a/kariwaza.xlsx
+++ b/kariwaza.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="171026"/>
 </workbook>
 </file>
 
@@ -28,73 +28,73 @@
     <t>condition</t>
   </si>
   <si>
-    <t>共通</t>
-  </si>
-  <si>
-    <t>絶対回避</t>
+    <t>공통</t>
+  </si>
+  <si>
+    <t>절대회피(絶対回避)</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>最初から</t>
-  </si>
-  <si>
-    <t>絶対回避【臨戦】</t>
+    <t>처음부터</t>
+  </si>
+  <si>
+    <t>절대회피【임전】(絶対回避【臨戦】)</t>
   </si>
   <si>
     <t>集★3砂上の竜脚</t>
   </si>
   <si>
-    <t>ヒールゲイン</t>
+    <t>힐게인(ヒールゲイン)</t>
   </si>
   <si>
     <t>村★3鬼面狩人を威す または 集★3電の反逆者</t>
   </si>
   <si>
-    <t>エスケープランナー</t>
-  </si>
-  <si>
-    <t>狩人のオアシス</t>
-  </si>
-  <si>
-    <t>ベルナ村の村人の依頼5回達成</t>
-  </si>
-  <si>
-    <t>完全調合</t>
-  </si>
-  <si>
-    <t>ポッケ村の村人の依頼5回達成</t>
-  </si>
-  <si>
-    <t>狂竜身</t>
+    <t>이스케이프 러너(エスケープランナー)</t>
+  </si>
+  <si>
+    <t>사냥꾼의 오아시스(狩人のオアシス)</t>
+  </si>
+  <si>
+    <t>베르나(ベルナ) 마을의 마을사람의 의뢰 5회 달성</t>
+  </si>
+  <si>
+    <t>완전조합(完全調合)</t>
+  </si>
+  <si>
+    <t>폿케(ポッケ) 마을의 마을사람의 의뢰 5회 달성</t>
+  </si>
+  <si>
+    <t>광룡신(狂竜身)</t>
   </si>
   <si>
     <t>集★6遺跡平原の黒蝕竜調査</t>
   </si>
   <si>
-    <t>鉄鋼身</t>
-  </si>
-  <si>
-    <t>ユクモ村の村人の依頼5回達成</t>
-  </si>
-  <si>
-    <t>金剛身</t>
+    <t>철강신(鉄鋼身)</t>
+  </si>
+  <si>
+    <t>유쿠모(ユクモ) 마을의 마을사람의 의뢰 5회 달성</t>
+  </si>
+  <si>
+    <t>금강신(金剛身)</t>
   </si>
   <si>
     <t>集★5脅威！火山の鉄槌！</t>
   </si>
   <si>
-    <t>不死鳥の息吹</t>
-  </si>
-  <si>
-    <t>ココット村の村人の依頼5回達成</t>
-  </si>
-  <si>
-    <t>大剣</t>
-  </si>
-  <si>
-    <t>地衝斬</t>
+    <t>불사조의 숨결(不死鳥の息吹)</t>
+  </si>
+  <si>
+    <t>코콧토(ココット) 마을의 마을사람의 의뢰 5회 달성</t>
+  </si>
+  <si>
+    <t>대검</t>
+  </si>
+  <si>
+    <t>지충참(地衝斬)</t>
   </si>
   <si>
     <t>LV1</t>
@@ -112,19 +112,19 @@
     <t>集★6砂漠の彼方から</t>
   </si>
   <si>
-    <t>獣宿し【獅子】</t>
+    <t>짐승깃들기【사자】(獣宿し【獅子】)</t>
   </si>
   <si>
     <t>村★2跳躍のアウトロー または 集★2雪山の主、ドドブランゴ</t>
   </si>
   <si>
-    <t>オトモアイルーのLV25以上</t>
+    <t>오토모아이루(オトモアイルー)의 LV25 이상</t>
   </si>
   <si>
     <t>集★7ビリビリバリバリパニック！！</t>
   </si>
   <si>
-    <t>震怒竜怨斬</t>
+    <t>진노용원참(震怒竜怨斬)</t>
   </si>
   <si>
     <t>村★6灼熱の刃</t>
@@ -133,7 +133,7 @@
     <t>集★7汝ノチカラヲ、見セテミヨ</t>
   </si>
   <si>
-    <t>ムーンブレイク</t>
+    <t>문브레이크(ムーンブレイク)</t>
   </si>
   <si>
     <t>村★7調査隊初陣！遺群嶺の桃毛獣 または 集★7その腕前、噂通りかしら…？</t>
@@ -145,16 +145,16 @@
     <t>G★4巨獣の進攻</t>
   </si>
   <si>
-    <t>太刀</t>
-  </si>
-  <si>
-    <t>桜花気刃斬</t>
+    <t>태도</t>
+  </si>
+  <si>
+    <t>앵화기인참(桜花気刃斬)</t>
   </si>
   <si>
     <t>集★7古の霞龍、オオナズチ</t>
   </si>
   <si>
-    <t>練気解放円月斬り</t>
+    <t>연기해방원월베기(練気解放円月斬り)</t>
   </si>
   <si>
     <t>集★3轟竜ティガレックス</t>
@@ -163,16 +163,16 @@
     <t>集★6狩られる前に狩れ！</t>
   </si>
   <si>
-    <t>鏡花の構え</t>
-  </si>
-  <si>
-    <t>ユクモ村の村貢献度400以上</t>
+    <t>경화의 자세(鏡花の構え)</t>
+  </si>
+  <si>
+    <t>유쿠모(ユクモ) 마을의 공헌도 400 이상</t>
   </si>
   <si>
     <t>集★7グランド・ハンター・ゲーム</t>
   </si>
   <si>
-    <t>妖刀羅刹</t>
+    <t>요도나찰(妖刀羅刹)</t>
   </si>
   <si>
     <t>G★2空の家族・空路を守るッス</t>
@@ -181,10 +181,10 @@
     <t>G★4風薫る密林</t>
   </si>
   <si>
-    <t>片手剣</t>
-  </si>
-  <si>
-    <t>ブレイドダンス</t>
+    <t>한손검</t>
+  </si>
+  <si>
+    <t>블레이드 댄스(ブレイドダンス)</t>
   </si>
   <si>
     <t>村★5怪鳥の頭部破壊に挑戦！ または 集★3双頭の骸</t>
@@ -193,22 +193,22 @@
     <t>集★7沼地酔夢譚</t>
   </si>
   <si>
-    <t>ラウンドフォース</t>
+    <t>라운드 포스(ラウンドフォース)</t>
   </si>
   <si>
     <t>集★5汗と涙の連続狩猟</t>
   </si>
   <si>
-    <t>昇竜撃</t>
-  </si>
-  <si>
-    <t>ココット村の村貢献度400以上</t>
+    <t>승룡격(昇竜撃)</t>
+  </si>
+  <si>
+    <t>코콧토(ココット) 마을의 공헌도 400 이상</t>
   </si>
   <si>
     <t>集★6スリルとショックの氷海ツアー</t>
   </si>
   <si>
-    <t>混沌の刃薬</t>
+    <t>혼돈의 인약(混沌の刃薬)</t>
   </si>
   <si>
     <t>G★2密林のナルガクルガと対峙せよ</t>
@@ -217,46 +217,46 @@
     <t>G★4金と銀がもたらす悲哀</t>
   </si>
   <si>
-    <t>双剣</t>
-  </si>
-  <si>
-    <t>血風独楽</t>
-  </si>
-  <si>
-    <t>天翔空破断</t>
-  </si>
-  <si>
-    <t>オトモアイルーのLV20以上</t>
+    <t>쌍검</t>
+  </si>
+  <si>
+    <t>혈풍독락(血風独楽)</t>
+  </si>
+  <si>
+    <t>천상공파단(天翔空破断)</t>
+  </si>
+  <si>
+    <t>오토모아이루(オトモアイルー)의 LV20 이상</t>
   </si>
   <si>
     <t>集★6狂乱の立体闘技場</t>
   </si>
   <si>
-    <t>獣宿し【餓狼】</t>
-  </si>
-  <si>
-    <t>イビルジョーを討伐</t>
+    <t>짐승깃들기【아랑】(獣宿し【餓狼】)</t>
+  </si>
+  <si>
+    <t>이빌죠(イビルジョー)를 토벌</t>
   </si>
   <si>
     <t>集★7憤怒の雄叫び</t>
   </si>
   <si>
-    <t>ラセンザン</t>
+    <t>나선참(ラセンザン)</t>
   </si>
   <si>
     <t>G★4焦電</t>
   </si>
   <si>
-    <t>ハンマー</t>
-  </si>
-  <si>
-    <t>スピニングメテオ</t>
+    <t>해머</t>
+  </si>
+  <si>
+    <t>스피닝 메테오(スピニングメテオ)</t>
   </si>
   <si>
     <t>集★6ドボルがために銅鑼は鳴る</t>
   </si>
   <si>
-    <t>大挑発</t>
+    <t>대도발(大挑発)</t>
   </si>
   <si>
     <t>集★5疾き迅竜の狩猟披露</t>
@@ -265,7 +265,7 @@
     <t>集★5グレート・ハンター・ゲーム</t>
   </si>
   <si>
-    <t>タイフーントリガー</t>
+    <t>타이푼 트리거(タイフーントリガー)</t>
   </si>
   <si>
     <t>村★5峨々たる巨獣</t>
@@ -274,7 +274,7 @@
     <t>集★7勇猛果敢なブレイブタスク</t>
   </si>
   <si>
-    <t>インパクトプルス</t>
+    <t>임팩트 펄스(インパクトプルス)</t>
   </si>
   <si>
     <t>G★2……欲するならば資格を示して</t>
@@ -283,13 +283,13 @@
     <t>G★4砂漠の死闘と未来</t>
   </si>
   <si>
-    <t>狩猟笛</t>
-  </si>
-  <si>
-    <t>オルケスタソウル</t>
-  </si>
-  <si>
-    <t>音撃震</t>
+    <t>수렵적</t>
+  </si>
+  <si>
+    <t>오르케스타 소울(オルケスタソウル)</t>
+  </si>
+  <si>
+    <t>음격진(音撃震)</t>
   </si>
   <si>
     <t>闘技大会★ガララアジャラ討伐</t>
@@ -298,7 +298,7 @@
     <t>集★7試練の帰結点</t>
   </si>
   <si>
-    <t>奏纏</t>
+    <t>주전(奏纏)</t>
   </si>
   <si>
     <t>集★4大地を泳ぐモンスター</t>
@@ -307,31 +307,31 @@
     <t>集★5毒、麻痺、混乱にご用心！</t>
   </si>
   <si>
-    <t>アニマートハイ</t>
+    <t>아니마토 하이(アニマートハイ)</t>
   </si>
   <si>
     <t>G★4狩魂よ砂中に眠れ</t>
   </si>
   <si>
-    <t>ランス</t>
-  </si>
-  <si>
-    <t>シールドアサルト</t>
+    <t>랜스</t>
+  </si>
+  <si>
+    <t>실드 어설트(シールドアサルト)</t>
   </si>
   <si>
     <t>集★5絞蛇竜は踊り奏でる</t>
   </si>
   <si>
-    <t>スクリュースラスト</t>
-  </si>
-  <si>
-    <t>ポッケ村の村貢献度400以上</t>
+    <t>스크류 스러스트(スクリュースラスト)</t>
+  </si>
+  <si>
+    <t>폿케(ポッケ)  마을의 공헌도 400 이상</t>
   </si>
   <si>
     <t>集★7氷点下の支配者</t>
   </si>
   <si>
-    <t>ガードレイジ</t>
+    <t>가드 레이지(ガードレイジ)</t>
   </si>
   <si>
     <t>集★3鎌将軍の包囲陣</t>
@@ -340,7 +340,7 @@
     <t>集★6原生林の曲者たち</t>
   </si>
   <si>
-    <t>治癒の盾</t>
+    <t>치유의 방패(治癒の盾)</t>
   </si>
   <si>
     <t>G★2依頼委託：火山の岩竜</t>
@@ -349,10 +349,10 @@
     <t>G★4シャル・ウィ・ダンス？</t>
   </si>
   <si>
-    <t>ガンランス</t>
-  </si>
-  <si>
-    <t>覇山竜撃砲</t>
+    <t>건랜스</t>
+  </si>
+  <si>
+    <t>패산용격포(覇山竜撃砲)</t>
   </si>
   <si>
     <t>集★3煉獄の主、怒れる炎帝</t>
@@ -361,10 +361,10 @@
     <t>集★7鎧袖一触のパワフルアームズ</t>
   </si>
   <si>
-    <t>ブラストダッシュ</t>
-  </si>
-  <si>
-    <t>竜の息吹</t>
+    <t>블러스트 대시(ブラストダッシュ)</t>
+  </si>
+  <si>
+    <t>용의 숨결(竜の息吹)</t>
   </si>
   <si>
     <t>村★5赤いおひさまアッチッチ</t>
@@ -373,19 +373,19 @@
     <t>集★7熱気で熱狂！炎の軍勢！</t>
   </si>
   <si>
-    <t>AAフレア</t>
+    <t>AA플레어(AAフレア)</t>
   </si>
   <si>
     <t>G★4死神は鎧をまとう</t>
   </si>
   <si>
-    <t>スラッシュアックス</t>
-  </si>
-  <si>
-    <t>トランスラッシュ</t>
-  </si>
-  <si>
-    <t>剣鬼形態</t>
+    <t>슬래시 액스</t>
+  </si>
+  <si>
+    <t>트랜슬래시(トランスラッシュ)</t>
+  </si>
+  <si>
+    <t>검귀형태(剣鬼形態)</t>
   </si>
   <si>
     <t>集★5壁に耳あり、天井に目あり？</t>
@@ -394,7 +394,7 @@
     <t>集★7破壊と滅亡の申し子</t>
   </si>
   <si>
-    <t>エネルギーチャージ</t>
+    <t>에네르기 차지(エネルギーチャージ)</t>
   </si>
   <si>
     <t>村★5混乱のホロロロホルルル</t>
@@ -403,7 +403,7 @@
     <t>集★6燃えたぎれ！火山の熱闘！！</t>
   </si>
   <si>
-    <t>テンペストアクス</t>
+    <t>템페스트 액스(テンペストアクス)</t>
   </si>
   <si>
     <t>G★2二人で特訓、成果は山分け</t>
@@ -412,43 +412,43 @@
     <t>G★4騎士と氷海の決闘</t>
   </si>
   <si>
-    <t>チャージアックス</t>
-  </si>
-  <si>
-    <t>エネルギーブレイド</t>
-  </si>
-  <si>
-    <t>キリンを討伐</t>
+    <t>차지 액스</t>
+  </si>
+  <si>
+    <t>에네르기 블레이드(エネルギーブレイド)</t>
+  </si>
+  <si>
+    <t>키린(キリン)을 토벌</t>
   </si>
   <si>
     <t>集★7震天動地なグランドウイング</t>
   </si>
   <si>
-    <t>オーバーリミット</t>
-  </si>
-  <si>
-    <t>ヒーリングボトル</t>
-  </si>
-  <si>
-    <t>ベルナ村の村貢献度400以上</t>
+    <t>오버 리미트(オーバーリミット)</t>
+  </si>
+  <si>
+    <t>힐링 보틀(ヒーリングボトル)</t>
+  </si>
+  <si>
+    <t>베르나(ベルナ) 마을의 공헌도 400 이상</t>
   </si>
   <si>
     <t>集★6飛竜たちの乱舞</t>
   </si>
   <si>
-    <t>チェインソーサー</t>
+    <t>체인 소서(チェインソーサー)</t>
   </si>
   <si>
     <t>G★4無心にて森羅万象を断つ</t>
   </si>
   <si>
-    <t>操虫棍</t>
-  </si>
-  <si>
-    <t>エキスハンター</t>
-  </si>
-  <si>
-    <t>蟲纏い</t>
+    <t>조충곤</t>
+  </si>
+  <si>
+    <t>엑스 헌터(エキスハンター)</t>
+  </si>
+  <si>
+    <t>벌레 두르기(蟲纏い)</t>
   </si>
   <si>
     <t>集★3狩られる前に狩れ！</t>
@@ -457,7 +457,7 @@
     <t>集★7まだ見ぬ秘湯をもとめて</t>
   </si>
   <si>
-    <t>飛翔蟲斬破</t>
+    <t>비상충참파(飛翔蟲斬破)</t>
   </si>
   <si>
     <t>集★4集いし強豪</t>
@@ -466,16 +466,16 @@
     <t>集★6沼地の狂騒楽団</t>
   </si>
   <si>
-    <t>覚蟲強化</t>
+    <t>각충강화(覚蟲強化)</t>
   </si>
   <si>
     <t>G★4天を廻りて、冥界に堕つ</t>
   </si>
   <si>
-    <t>ライトボウガン</t>
-  </si>
-  <si>
-    <t>バレットゲイザー</t>
+    <t>라이트 보우건</t>
+  </si>
+  <si>
+    <t>블릿 게이저(バレットゲイザー)</t>
   </si>
   <si>
     <t>村★5翠玉の閃電</t>
@@ -484,10 +484,10 @@
     <t>集★7森丘の黒い霧</t>
   </si>
   <si>
-    <t>全弾装填</t>
-  </si>
-  <si>
-    <t>ラピッドヘブン</t>
+    <t>전탄장전(全弾装填)</t>
+  </si>
+  <si>
+    <t>래피드 헤븐(ラピッドヘブン)</t>
   </si>
   <si>
     <t>集★3廻り集いて回帰せん</t>
@@ -496,7 +496,7 @@
     <t>集★7住めば都の闘技場暮らし</t>
   </si>
   <si>
-    <t>チャージショット</t>
+    <t>차지 샷(チャージショット)</t>
   </si>
   <si>
     <t>G★2閃きへの1ピースを求めて</t>
@@ -505,10 +505,10 @@
     <t>G★4溶岩島で爆ぜる砕光</t>
   </si>
   <si>
-    <t>ヘビィボウガン</t>
-  </si>
-  <si>
-    <t>スーパーノヴァ</t>
+    <t>헤비 보우건</t>
+  </si>
+  <si>
+    <t>슈퍼 노바(スーパーノヴァ)</t>
   </si>
   <si>
     <t>村★6粉骨砕竜！</t>
@@ -517,7 +517,7 @@
     <t>集★7煉獄の主、怒れる炎帝</t>
   </si>
   <si>
-    <t>アクセルシャワー</t>
+    <t>액셀 샤워(アクセルシャワー)</t>
   </si>
   <si>
     <t>村★5淡紅の泡狐がたゆたうか</t>
@@ -526,34 +526,34 @@
     <t>集★5不眠のあなたに催眠療法×２</t>
   </si>
   <si>
-    <t>火薬装填</t>
+    <t>화약장전(火薬装填)</t>
   </si>
   <si>
     <t>集★6地底火山に響く侵略の足音</t>
   </si>
   <si>
-    <t>射突型裂孔弾</t>
+    <t>사돌형열공탄(射突型裂孔弾)</t>
   </si>
   <si>
     <t>G★4戦慄の遺群嶺</t>
   </si>
   <si>
-    <t>弓</t>
-  </si>
-  <si>
-    <t>トリニティレイヴン</t>
+    <t>활</t>
+  </si>
+  <si>
+    <t>트리니티 레이븐(トリニティレイヴン)</t>
   </si>
   <si>
     <t>集★7奇奇怪怪のハードビーク</t>
   </si>
   <si>
-    <t>アクセルレイン</t>
+    <t>액셀 레인(アクセルレイン)</t>
   </si>
   <si>
     <t>闘技大会★ケチャワチャ討伐</t>
   </si>
   <si>
-    <t>ブレイドワイヤー</t>
+    <t>블레이드 와이어(ブレイドワイヤー)</t>
   </si>
   <si>
     <t>村★6青と緑の波状包囲網 または 集★5渓流の水竜</t>
@@ -562,7 +562,7 @@
     <t>集★6ワイルドバレット</t>
   </si>
   <si>
-    <t>身躱し射法</t>
+    <t>회피사법(身躱し射法)</t>
   </si>
   <si>
     <t>G★4金色超巨星</t>
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -605,10 +605,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -655,7 +663,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -687,9 +695,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,6 +747,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -896,12 +940,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="D128" sqref="D128"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">

</xml_diff>